<commit_message>
Initial version of working model (converges)
</commit_message>
<xml_diff>
--- a/data/Beluga_data.xlsx
+++ b/data/Beluga_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/26362cec7e0913ab/Documents/Nhydra/Projects/Beluga/Belugamod/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="30" documentId="8_{40E31F02-9A58-48C7-B6F0-DAB028A2CBEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{80E259EB-14E9-496D-BF52-5518A7F98238}"/>
+  <xr:revisionPtr revIDLastSave="80" documentId="8_{40E31F02-9A58-48C7-B6F0-DAB028A2CBEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F8BE1828-6D5F-4794-9C81-CD9EFFC50A44}"/>
   <bookViews>
-    <workbookView xWindow="30225" yWindow="195" windowWidth="27015" windowHeight="14535" tabRatio="734" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="570" yWindow="315" windowWidth="27015" windowHeight="14535" tabRatio="734" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Initial vector" sheetId="3" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="14">
   <si>
     <t>Age</t>
   </si>
@@ -74,6 +74,12 @@
   </si>
   <si>
     <t>Prop_juv</t>
+  </si>
+  <si>
+    <t>SE</t>
+  </si>
+  <si>
+    <t>Old_mod_est</t>
   </si>
 </sst>
 </file>
@@ -115,9 +121,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -400,11 +407,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.140625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -919,10 +929,13 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="7.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -1027,60 +1040,79 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
       <c r="B1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1988</v>
       </c>
       <c r="B2">
+        <v>893</v>
+      </c>
+      <c r="C2">
+        <v>178.6</v>
+      </c>
+      <c r="D2" s="1">
+        <v>0.1678</v>
+      </c>
+      <c r="E2">
         <v>898</v>
       </c>
-      <c r="C2">
+      <c r="F2">
         <v>36.159999999999997</v>
       </c>
-      <c r="D2" s="1">
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1990</v>
       </c>
       <c r="B3">
+        <v>1129</v>
+      </c>
+      <c r="C3">
+        <v>564.5</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0.1678</v>
+      </c>
+      <c r="E3">
         <v>1106</v>
       </c>
-      <c r="C3">
+      <c r="F3">
         <v>2.2000000000000002</v>
       </c>
-      <c r="D3" s="1">
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1992</v>
       </c>
@@ -1088,13 +1120,19 @@
         <v>952</v>
       </c>
       <c r="C4">
+        <v>152.32</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0.16300000000000001</v>
+      </c>
+      <c r="E4">
+        <v>952</v>
+      </c>
+      <c r="F4">
         <v>38.159999999999997</v>
       </c>
-      <c r="D4" s="1">
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1995</v>
       </c>
@@ -1102,13 +1140,19 @@
         <v>1239</v>
       </c>
       <c r="C5">
+        <v>223.02</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0.15140000000000001</v>
+      </c>
+      <c r="E5">
+        <v>1239</v>
+      </c>
+      <c r="F5">
         <v>29.9</v>
       </c>
-      <c r="D5" s="1">
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1997</v>
       </c>
@@ -1116,13 +1160,19 @@
         <v>1222</v>
       </c>
       <c r="C6">
+        <v>195.52</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0.1777</v>
+      </c>
+      <c r="E6">
+        <v>1222</v>
+      </c>
+      <c r="F6">
         <v>38.770000000000003</v>
       </c>
-      <c r="D6" s="1">
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2000</v>
       </c>
@@ -1130,13 +1180,19 @@
         <v>953</v>
       </c>
       <c r="C7">
+        <v>133.41999999999999</v>
+      </c>
+      <c r="D7" s="2">
+        <v>7.7600000000000002E-2</v>
+      </c>
+      <c r="E7">
+        <v>953</v>
+      </c>
+      <c r="F7">
         <v>48.03</v>
       </c>
-      <c r="D7" s="1">
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2003</v>
       </c>
@@ -1144,13 +1200,19 @@
         <v>1319</v>
       </c>
       <c r="C8">
+        <v>263.8</v>
+      </c>
+      <c r="D8" s="2">
+        <v>3.2199999999999999E-2</v>
+      </c>
+      <c r="E8">
+        <v>1319</v>
+      </c>
+      <c r="F8">
         <v>22.44</v>
       </c>
-      <c r="D8" s="1">
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2009</v>
       </c>
@@ -1158,10 +1220,16 @@
         <v>676</v>
       </c>
       <c r="C9">
+        <v>108.16</v>
+      </c>
+      <c r="D9" s="2">
+        <v>8.4399999999999989E-2</v>
+      </c>
+      <c r="E9">
+        <v>676</v>
+      </c>
+      <c r="F9">
         <v>38.76</v>
-      </c>
-      <c r="D9" s="1">
-        <v>0.15</v>
       </c>
     </row>
   </sheetData>
@@ -1175,7 +1243,7 @@
   <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added stranded animal age distributions
</commit_message>
<xml_diff>
--- a/data/Beluga_data.xlsx
+++ b/data/Beluga_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/26362cec7e0913ab/Documents/Nhydra/Projects/Beluga/Belugamod/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="80" documentId="8_{40E31F02-9A58-48C7-B6F0-DAB028A2CBEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F8BE1828-6D5F-4794-9C81-CD9EFFC50A44}"/>
+  <xr:revisionPtr revIDLastSave="86" documentId="8_{40E31F02-9A58-48C7-B6F0-DAB028A2CBEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{53CFC85E-585C-46D4-ABAB-A6DC367A86E1}"/>
   <bookViews>
-    <workbookView xWindow="570" yWindow="315" windowWidth="27015" windowHeight="14535" tabRatio="734" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="734" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Initial vector" sheetId="3" r:id="rId1"/>
@@ -407,7 +407,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
@@ -1242,8 +1242,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added second version of model that does not use carcass age data for fitting (fit to same data as JAGS model)
</commit_message>
<xml_diff>
--- a/data/Beluga_data.xlsx
+++ b/data/Beluga_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/26362cec7e0913ab/Documents/Nhydra/Projects/Beluga/Belugamod/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="86" documentId="8_{40E31F02-9A58-48C7-B6F0-DAB028A2CBEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{53CFC85E-585C-46D4-ABAB-A6DC367A86E1}"/>
+  <xr:revisionPtr revIDLastSave="98" documentId="8_{40E31F02-9A58-48C7-B6F0-DAB028A2CBEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EF5EB35C-9BDE-40B0-8CF9-B8E7724F4855}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="734" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29925" yWindow="315" windowWidth="27465" windowHeight="14910" tabRatio="734" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Initial vector" sheetId="3" r:id="rId1"/>
@@ -1243,7 +1243,7 @@
   <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+      <selection activeCell="E34" sqref="A33:E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1295,11 +1295,11 @@
         <v>13</v>
       </c>
       <c r="D3">
-        <f>ROUND(B3*0.8,0)+ROUND(B2*0.2,0)</f>
+        <f>ROUND(B3*0.83,0)+ROUND(B2*0.17,0)</f>
         <v>2</v>
       </c>
       <c r="E3">
-        <f>ROUND(C3*0.8,0)+ROUND(C2*0.2,0)</f>
+        <f>ROUND(C3*0.72,0)+ROUND(C2*0.28,0)</f>
         <v>12</v>
       </c>
     </row>
@@ -1314,11 +1314,11 @@
         <v>12</v>
       </c>
       <c r="D4">
-        <f t="shared" ref="D4:E32" si="0">ROUND(B4*0.8,0)+ROUND(B3*0.2,0)</f>
+        <f t="shared" ref="D4:D32" si="0">ROUND(B4*0.83,0)+ROUND(B3*0.17,0)</f>
         <v>0</v>
       </c>
       <c r="E4">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="E4:E32" si="1">ROUND(C4*0.72,0)+ROUND(C3*0.28,0)</f>
         <v>13</v>
       </c>
     </row>
@@ -1337,7 +1337,7 @@
         <v>0</v>
       </c>
       <c r="E5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
     </row>
@@ -1356,7 +1356,7 @@
         <v>1</v>
       </c>
       <c r="E6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
     </row>
@@ -1375,7 +1375,7 @@
         <v>1</v>
       </c>
       <c r="E7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
     </row>
@@ -1394,7 +1394,7 @@
         <v>2</v>
       </c>
       <c r="E8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>16</v>
       </c>
     </row>
@@ -1413,7 +1413,7 @@
         <v>1</v>
       </c>
       <c r="E9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>19</v>
       </c>
     </row>
@@ -1432,7 +1432,7 @@
         <v>1</v>
       </c>
       <c r="E10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>17</v>
       </c>
     </row>
@@ -1451,7 +1451,7 @@
         <v>2</v>
       </c>
       <c r="E11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>14</v>
       </c>
     </row>
@@ -1470,7 +1470,7 @@
         <v>2</v>
       </c>
       <c r="E12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>14</v>
       </c>
     </row>
@@ -1489,8 +1489,8 @@
         <v>0</v>
       </c>
       <c r="E13">
-        <f t="shared" si="0"/>
-        <v>19</v>
+        <f t="shared" si="1"/>
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -1508,8 +1508,8 @@
         <v>0</v>
       </c>
       <c r="E14">
-        <f t="shared" si="0"/>
-        <v>14</v>
+        <f t="shared" si="1"/>
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -1527,7 +1527,7 @@
         <v>2</v>
       </c>
       <c r="E15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>13</v>
       </c>
     </row>
@@ -1546,7 +1546,7 @@
         <v>1</v>
       </c>
       <c r="E16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
     </row>
@@ -1565,7 +1565,7 @@
         <v>1</v>
       </c>
       <c r="E17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>13</v>
       </c>
     </row>
@@ -1584,7 +1584,7 @@
         <v>0</v>
       </c>
       <c r="E18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>13</v>
       </c>
     </row>
@@ -1603,7 +1603,7 @@
         <v>2</v>
       </c>
       <c r="E19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>14</v>
       </c>
     </row>
@@ -1622,7 +1622,7 @@
         <v>2</v>
       </c>
       <c r="E20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>13</v>
       </c>
     </row>
@@ -1641,7 +1641,7 @@
         <v>0</v>
       </c>
       <c r="E21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
     </row>
@@ -1660,7 +1660,7 @@
         <v>1</v>
       </c>
       <c r="E22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
     </row>
@@ -1679,7 +1679,7 @@
         <v>2</v>
       </c>
       <c r="E23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>13</v>
       </c>
     </row>
@@ -1698,7 +1698,7 @@
         <v>1</v>
       </c>
       <c r="E24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>17</v>
       </c>
     </row>
@@ -1717,7 +1717,7 @@
         <v>0</v>
       </c>
       <c r="E25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
     </row>
@@ -1736,7 +1736,7 @@
         <v>0</v>
       </c>
       <c r="E26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
     </row>
@@ -1755,7 +1755,7 @@
         <v>2</v>
       </c>
       <c r="E27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>13</v>
       </c>
     </row>
@@ -1771,10 +1771,10 @@
       </c>
       <c r="D28">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>16</v>
       </c>
     </row>
@@ -1790,10 +1790,10 @@
       </c>
       <c r="D29">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>13</v>
       </c>
     </row>
@@ -1808,10 +1808,11 @@
         <v>14</v>
       </c>
       <c r="D30">
-        <v>7</v>
+        <f>B30</f>
+        <v>8</v>
       </c>
       <c r="E30">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>14</v>
       </c>
     </row>
@@ -1827,10 +1828,10 @@
       </c>
       <c r="D31">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
     </row>
@@ -1845,10 +1846,11 @@
         <v>12</v>
       </c>
       <c r="D32">
+        <f>B32</f>
         <v>16</v>
       </c>
       <c r="E32">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
     </row>

</xml_diff>